<commit_message>
created method to read/write data from csv file
Added Navigation Test script tc006-tc008

Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/TestCases - Copy.xlsx
+++ b/TestCases - Copy.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Modules" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCases" sheetId="10" r:id="rId2"/>
-    <sheet name="Users" sheetId="3" r:id="rId3"/>
+    <sheet name="Modules" r:id="rId1" sheetId="1"/>
+    <sheet name="TestCases" r:id="rId2" sheetId="10"/>
+    <sheet name="Users" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="108">
   <si>
     <t>Module_Name</t>
   </si>
@@ -277,9 +277,6 @@
     <t>FSTc015_createFieldsForPackageObject</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>FSTc014_CreatedataForPackageObject</t>
   </si>
   <si>
@@ -329,12 +326,44 @@
   </si>
   <si>
     <t>Module3Tc001_createCRMUser</t>
+  </si>
+  <si>
+    <t>FSTc018_verifyFieldSetImagePath</t>
+  </si>
+  <si>
+    <t>FSTc019_addProfileImageFieldOnLayOut</t>
+  </si>
+  <si>
+    <t>Module3</t>
+  </si>
+  <si>
+    <t>Module3Tc004_OpentheNavigationMenuAndVerifyTheMenuItems</t>
+  </si>
+  <si>
+    <t>Fail: timeout: Timed out receiving message from renderer: 10.000
+  (Session info: chrome=88.0.4324.104)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:25:53'
+System info: host: 'DESKTOP-K4MTBVJ', ip: '192.168.0.104', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_141'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 88.0.4324.104, chrome: {chromedriverVersion: 87.0.4280.20 (c99e81631faa0..., userDataDir: C:\Users\sibaram\AppData\Lo...}, goog:chromeOptions: {debuggerAddress: localhost:63888}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:virtualAuthenticators: true}
+Session ID: 1b41886e1662c3724adefb794bc06a38</t>
+  </si>
+  <si>
+    <t>Module3Tc005_VerifyTheURLNavigationFromNavigationMenu</t>
+  </si>
+  <si>
+    <t>Fail: 7</t>
+  </si>
+  <si>
+    <t>Fail: The following asserts failed:
+	Url Not Verified for : Navatar Setup Actual : https://pe4604.lightning.force.com/lightning/page/home	 Expected : /lightning/n/navmnaI__Navatar_Setup (Module3.java:434)	Screenshot Name: Module3Tc005_VerifyTheURLNavigationFromNavigationMenu2021_02_05_06_50_23.png	 did not expect to find [true] but found [false]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -507,63 +536,207 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle name="Hyperlink 2" xfId="2"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="325">
+  <dxfs count="342">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -592,6 +765,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -718,6 +918,78 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -916,6 +1188,87 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1015,6 +1368,150 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -1069,6 +1566,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3772,320 +4296,19 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9D18E"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -4170,10 +4393,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -4208,7 +4431,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4243,7 +4466,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4337,21 +4560,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -4368,7 +4591,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -4420,29 +4643,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H1:J5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="7" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="1025" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row ht="15.75" r="1" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4450,15 +4673,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row ht="15.75" r="3" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
@@ -4466,7 +4689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="4" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H4" s="2" t="s">
         <v>30</v>
       </c>
@@ -4474,56 +4697,74 @@
         <v>7</v>
       </c>
     </row>
+    <row ht="15.75" r="5" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="294" priority="6" operator="equal">
+    <cfRule dxfId="341" operator="equal" priority="8" type="cellIs">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="293" priority="7" operator="equal">
+    <cfRule dxfId="340" operator="equal" priority="9" type="cellIs">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="292" priority="1" operator="equal">
+    <cfRule dxfId="339" operator="equal" priority="3" type="cellIs">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="291" priority="2" operator="equal">
+    <cfRule dxfId="338" operator="equal" priority="4" type="cellIs">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule dxfId="337" operator="equal" priority="1" type="cellIs">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule dxfId="336" operator="equal" priority="2" type="cellIs">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I4">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="I2:I5" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="87.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="18" r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -4540,7 +4781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>36</v>
       </c>
@@ -4555,7 +4796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -4570,7 +4811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
@@ -4585,7 +4826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>39</v>
       </c>
@@ -4600,7 +4841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
@@ -4615,7 +4856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>48</v>
       </c>
@@ -4630,7 +4871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
@@ -4645,7 +4886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>50</v>
       </c>
@@ -4660,7 +4901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
@@ -4675,7 +4916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>52</v>
       </c>
@@ -4690,7 +4931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>53</v>
       </c>
@@ -4705,7 +4946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>54</v>
       </c>
@@ -4720,7 +4961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="14" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>55</v>
       </c>
@@ -4735,7 +4976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="15" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>66</v>
       </c>
@@ -4750,7 +4991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="16" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>67</v>
       </c>
@@ -4765,7 +5006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="17" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>68</v>
       </c>
@@ -4780,7 +5021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="18" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>69</v>
       </c>
@@ -4795,7 +5036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="19" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>70</v>
       </c>
@@ -4810,7 +5051,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="20" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>71</v>
       </c>
@@ -4825,7 +5066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="21" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>72</v>
       </c>
@@ -4840,7 +5081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="22" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>73</v>
       </c>
@@ -4855,7 +5096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="23" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>74</v>
       </c>
@@ -4870,7 +5111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="24" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>75</v>
       </c>
@@ -4885,7 +5126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="25" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>76</v>
       </c>
@@ -4900,7 +5141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="26" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>77</v>
       </c>
@@ -4915,9 +5156,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="27" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="3" t="s">
@@ -4930,9 +5171,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="28" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="3" t="s">
@@ -4945,9 +5186,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="29" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="3" t="s">
@@ -4960,9 +5201,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="30" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="3" t="s">
@@ -4975,9 +5216,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="31" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="3" t="s">
@@ -4990,9 +5231,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="32" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="3" t="s">
@@ -5005,9 +5246,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="33" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="3" t="s">
@@ -5020,7 +5261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="34" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>31</v>
       </c>
@@ -5037,7 +5278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="35" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>32</v>
       </c>
@@ -5054,7 +5295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="36" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>33</v>
       </c>
@@ -5071,7 +5312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="37" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>34</v>
       </c>
@@ -5088,9 +5329,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="38" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="8">
         <v>1</v>
@@ -5105,7 +5346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="39" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>43</v>
       </c>
@@ -5122,7 +5363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="40" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>42</v>
       </c>
@@ -5139,7 +5380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="41" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>44</v>
       </c>
@@ -5156,9 +5397,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="42" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="8">
         <v>1</v>
@@ -5173,9 +5414,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="43" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" s="8">
         <v>1</v>
@@ -5190,9 +5431,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="44" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B44" s="8">
         <v>1</v>
@@ -5207,11 +5448,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="45" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B45" s="8"/>
+        <v>99</v>
+      </c>
+      <c r="B45" s="8">
+        <v>1</v>
+      </c>
       <c r="C45" s="3" t="s">
         <v>7</v>
       </c>
@@ -5222,12 +5465,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="46" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>7</v>
@@ -5239,12 +5482,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="47" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>7</v>
@@ -5256,12 +5499,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="14" t="s">
+    <row customHeight="1" ht="15" r="48" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="8">
+        <v>4</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D48" t="s">
@@ -5271,24 +5516,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="49" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="14" t="s">
-        <v>7</v>
+        <v>105</v>
+      </c>
+      <c r="B49" s="8">
+        <v>4</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>47</v>
+    <row customHeight="1" ht="15" r="50" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="14" t="s">
@@ -5301,9 +5548,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="51" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="14" t="s">
@@ -5316,9 +5563,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="52" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="14" t="s">
@@ -5331,9 +5578,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="53" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="14" t="s">
@@ -5346,9 +5593,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="54" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="14" t="s">
@@ -5361,9 +5608,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="55" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="14" t="s">
@@ -5376,9 +5623,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="56" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="14" t="s">
@@ -5391,9 +5638,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="57" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="14" t="s">
@@ -5406,9 +5653,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="58" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="14" t="s">
@@ -5421,9 +5668,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="59" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="14" t="s">
@@ -5436,9 +5683,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="60" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="14" t="s">
@@ -5451,9 +5698,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="61" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="14" t="s">
@@ -5466,9 +5713,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="16" t="s">
-        <v>84</v>
+    <row customHeight="1" ht="15" r="62" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="14" t="s">
@@ -5481,9 +5728,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>82</v>
+    <row customHeight="1" ht="15" r="63" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="14" t="s">
@@ -5496,9 +5743,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>92</v>
+    <row customHeight="1" ht="15" r="64" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
+        <v>83</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="14" t="s">
@@ -5511,1121 +5758,1313 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="65" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>9</v>
       </c>
     </row>
+    <row customHeight="1" ht="15" r="66" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="67" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>92</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="68" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="69" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E6 E45">
-    <cfRule type="cellIs" dxfId="290" priority="355" operator="equal">
+    <cfRule dxfId="335" operator="equal" priority="397" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="289" priority="356" operator="equal">
+    <cfRule dxfId="334" operator="equal" priority="398" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="288" priority="357" operator="equal">
+    <cfRule dxfId="333" operator="equal" priority="399" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2 D44:D45">
-    <cfRule type="containsText" dxfId="287" priority="394" operator="containsText" text="Skip:">
+    <cfRule dxfId="332" operator="containsText" priority="436" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="286" priority="395" operator="containsText" text="Fail">
+    <cfRule dxfId="331" operator="containsText" priority="437" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="396" operator="containsText" text="Pass">
+    <cfRule dxfId="330" operator="containsText" priority="438" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="284" priority="397" operator="containsText" text="Skip:">
+    <cfRule dxfId="329" operator="containsText" priority="439" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="283" priority="398" operator="containsText" text="Fail">
+    <cfRule dxfId="328" operator="containsText" priority="440" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="399" operator="containsText" text="Pass">
+    <cfRule dxfId="327" operator="containsText" priority="441" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="281" priority="388" operator="containsText" text="Skip:">
+    <cfRule dxfId="326" operator="containsText" priority="430" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="280" priority="389" operator="containsText" text="Fail">
+    <cfRule dxfId="325" operator="containsText" priority="431" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="279" priority="390" operator="containsText" text="Pass">
+    <cfRule dxfId="324" operator="containsText" priority="432" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="278" priority="391" operator="containsText" text="Skip:">
+    <cfRule dxfId="323" operator="containsText" priority="433" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="392" operator="containsText" text="Fail">
+    <cfRule dxfId="322" operator="containsText" priority="434" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="276" priority="393" operator="containsText" text="Pass">
+    <cfRule dxfId="321" operator="containsText" priority="435" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="275" priority="382" operator="containsText" text="Skip:">
+    <cfRule dxfId="320" operator="containsText" priority="424" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="274" priority="383" operator="containsText" text="Fail">
+    <cfRule dxfId="319" operator="containsText" priority="425" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="384" operator="containsText" text="Pass">
+    <cfRule dxfId="318" operator="containsText" priority="426" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="272" priority="385" operator="containsText" text="Skip:">
+    <cfRule dxfId="317" operator="containsText" priority="427" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="271" priority="386" operator="containsText" text="Fail">
+    <cfRule dxfId="316" operator="containsText" priority="428" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="387" operator="containsText" text="Pass">
+    <cfRule dxfId="315" operator="containsText" priority="429" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="269" priority="376" operator="containsText" text="Skip:">
+    <cfRule dxfId="314" operator="containsText" priority="418" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="268" priority="377" operator="containsText" text="Fail">
+    <cfRule dxfId="313" operator="containsText" priority="419" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="267" priority="378" operator="containsText" text="Pass">
+    <cfRule dxfId="312" operator="containsText" priority="420" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="266" priority="379" operator="containsText" text="Skip:">
+    <cfRule dxfId="311" operator="containsText" priority="421" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="380" operator="containsText" text="Fail">
+    <cfRule dxfId="310" operator="containsText" priority="422" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="264" priority="381" operator="containsText" text="Pass">
+    <cfRule dxfId="309" operator="containsText" priority="423" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="263" priority="370" operator="containsText" text="Skip:">
+    <cfRule dxfId="308" operator="containsText" priority="412" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="371" operator="containsText" text="Fail">
+    <cfRule dxfId="307" operator="containsText" priority="413" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="372" operator="containsText" text="Pass">
+    <cfRule dxfId="306" operator="containsText" priority="414" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="260" priority="373" operator="containsText" text="Skip:">
+    <cfRule dxfId="305" operator="containsText" priority="415" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="259" priority="374" operator="containsText" text="Fail">
+    <cfRule dxfId="304" operator="containsText" priority="416" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="375" operator="containsText" text="Pass">
+    <cfRule dxfId="303" operator="containsText" priority="417" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="257" priority="367" operator="equal">
+    <cfRule dxfId="302" operator="equal" priority="409" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="256" priority="368" operator="equal">
+    <cfRule dxfId="301" operator="equal" priority="410" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="255" priority="369" operator="equal">
+    <cfRule dxfId="300" operator="equal" priority="411" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="254" priority="364" operator="equal">
+    <cfRule dxfId="299" operator="equal" priority="406" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="365" operator="equal">
+    <cfRule dxfId="298" operator="equal" priority="407" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="252" priority="366" operator="equal">
+    <cfRule dxfId="297" operator="equal" priority="408" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="251" priority="361" operator="equal">
+    <cfRule dxfId="296" operator="equal" priority="403" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="362" operator="equal">
+    <cfRule dxfId="295" operator="equal" priority="404" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="249" priority="363" operator="equal">
+    <cfRule dxfId="294" operator="equal" priority="405" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="248" priority="358" operator="equal">
+    <cfRule dxfId="293" operator="equal" priority="400" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="359" operator="equal">
+    <cfRule dxfId="292" operator="equal" priority="401" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="360" operator="equal">
+    <cfRule dxfId="291" operator="equal" priority="402" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="245" priority="250" operator="containsText" text="Skip:">
+    <cfRule dxfId="290" operator="containsText" priority="292" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="244" priority="251" operator="containsText" text="Fail">
+    <cfRule dxfId="289" operator="containsText" priority="293" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="243" priority="252" operator="containsText" text="Pass">
+    <cfRule dxfId="288" operator="containsText" priority="294" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="242" priority="253" operator="containsText" text="Skip:">
+    <cfRule dxfId="287" operator="containsText" priority="295" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="254" operator="containsText" text="Fail">
+    <cfRule dxfId="286" operator="containsText" priority="296" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="240" priority="255" operator="containsText" text="Pass">
+    <cfRule dxfId="285" operator="containsText" priority="297" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="239" priority="247" operator="equal">
+    <cfRule dxfId="284" operator="equal" priority="289" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="248" operator="equal">
+    <cfRule dxfId="283" operator="equal" priority="290" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="249" operator="equal">
+    <cfRule dxfId="282" operator="equal" priority="291" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D50">
-    <cfRule type="containsText" dxfId="236" priority="319" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D50:D52">
+    <cfRule dxfId="281" operator="containsText" priority="361" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D50)))</formula>
+    </cfRule>
+    <cfRule dxfId="280" operator="containsText" priority="362" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D50)))</formula>
+    </cfRule>
+    <cfRule dxfId="279" operator="containsText" priority="363" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50:D52">
+    <cfRule dxfId="278" operator="containsText" priority="364" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D50)))</formula>
+    </cfRule>
+    <cfRule dxfId="277" operator="containsText" priority="365" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D50)))</formula>
+    </cfRule>
+    <cfRule dxfId="276" operator="containsText" priority="366" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:E33">
+    <cfRule dxfId="275" operator="equal" priority="280" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="274" operator="equal" priority="281" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="273" operator="equal" priority="282" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:E52">
+    <cfRule dxfId="272" operator="equal" priority="322" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="271" operator="equal" priority="323" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="270" operator="equal" priority="324" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
+    <cfRule dxfId="269" operator="equal" priority="235" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="268" operator="equal" priority="236" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="267" operator="equal" priority="237" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D33">
+    <cfRule dxfId="266" operator="containsText" priority="283" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="265" operator="containsText" priority="284" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="264" operator="containsText" priority="285" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D33">
+    <cfRule dxfId="263" operator="containsText" priority="286" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="262" operator="containsText" priority="287" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="261" operator="containsText" priority="288" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule dxfId="260" operator="containsText" priority="265" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D53)))</formula>
+    </cfRule>
+    <cfRule dxfId="259" operator="containsText" priority="266" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D53)))</formula>
+    </cfRule>
+    <cfRule dxfId="258" operator="containsText" priority="267" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule dxfId="257" operator="containsText" priority="268" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D53)))</formula>
+    </cfRule>
+    <cfRule dxfId="256" operator="containsText" priority="269" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D53)))</formula>
+    </cfRule>
+    <cfRule dxfId="255" operator="containsText" priority="270" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule dxfId="254" operator="equal" priority="262" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="253" operator="equal" priority="263" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="252" operator="equal" priority="264" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule dxfId="251" operator="containsText" priority="256" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D54)))</formula>
+    </cfRule>
+    <cfRule dxfId="250" operator="containsText" priority="257" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D54)))</formula>
+    </cfRule>
+    <cfRule dxfId="249" operator="containsText" priority="258" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule dxfId="248" operator="containsText" priority="259" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D54)))</formula>
+    </cfRule>
+    <cfRule dxfId="247" operator="containsText" priority="260" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D54)))</formula>
+    </cfRule>
+    <cfRule dxfId="246" operator="containsText" priority="261" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54">
+    <cfRule dxfId="245" operator="equal" priority="253" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="244" operator="equal" priority="254" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="243" operator="equal" priority="255" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule dxfId="242" operator="containsText" priority="247" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D55)))</formula>
+    </cfRule>
+    <cfRule dxfId="241" operator="containsText" priority="248" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D55)))</formula>
+    </cfRule>
+    <cfRule dxfId="240" operator="containsText" priority="249" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule dxfId="239" operator="containsText" priority="250" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D55)))</formula>
+    </cfRule>
+    <cfRule dxfId="238" operator="containsText" priority="251" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D55)))</formula>
+    </cfRule>
+    <cfRule dxfId="237" operator="containsText" priority="252" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule dxfId="236" operator="equal" priority="244" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="235" operator="equal" priority="245" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="234" operator="equal" priority="246" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule dxfId="233" operator="containsText" priority="238" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D56)))</formula>
+    </cfRule>
+    <cfRule dxfId="232" operator="containsText" priority="239" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D56)))</formula>
+    </cfRule>
+    <cfRule dxfId="231" operator="containsText" priority="240" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule dxfId="230" operator="containsText" priority="241" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D56)))</formula>
+    </cfRule>
+    <cfRule dxfId="229" operator="containsText" priority="242" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D56)))</formula>
+    </cfRule>
+    <cfRule dxfId="228" operator="containsText" priority="243" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule dxfId="227" operator="containsText" priority="229" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D57)))</formula>
+    </cfRule>
+    <cfRule dxfId="226" operator="containsText" priority="230" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D57)))</formula>
+    </cfRule>
+    <cfRule dxfId="225" operator="containsText" priority="231" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule dxfId="224" operator="containsText" priority="232" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D57)))</formula>
+    </cfRule>
+    <cfRule dxfId="223" operator="containsText" priority="233" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D57)))</formula>
+    </cfRule>
+    <cfRule dxfId="222" operator="containsText" priority="234" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule dxfId="221" operator="equal" priority="226" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="220" operator="equal" priority="227" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="219" operator="equal" priority="228" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule dxfId="218" operator="containsText" priority="220" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
+    </cfRule>
+    <cfRule dxfId="217" operator="containsText" priority="221" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
+    </cfRule>
+    <cfRule dxfId="216" operator="containsText" priority="222" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule dxfId="215" operator="containsText" priority="223" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
+    </cfRule>
+    <cfRule dxfId="214" operator="containsText" priority="224" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
+    </cfRule>
+    <cfRule dxfId="213" operator="containsText" priority="225" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule dxfId="212" operator="equal" priority="217" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="211" operator="equal" priority="218" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="210" operator="equal" priority="219" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule dxfId="209" operator="containsText" priority="211" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
+    </cfRule>
+    <cfRule dxfId="208" operator="containsText" priority="212" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
+    </cfRule>
+    <cfRule dxfId="207" operator="containsText" priority="213" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule dxfId="206" operator="containsText" priority="214" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
+    </cfRule>
+    <cfRule dxfId="205" operator="containsText" priority="215" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
+    </cfRule>
+    <cfRule dxfId="204" operator="containsText" priority="216" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule dxfId="203" operator="equal" priority="208" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="202" operator="equal" priority="209" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="201" operator="equal" priority="210" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule dxfId="200" operator="containsText" priority="202" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D60)))</formula>
+    </cfRule>
+    <cfRule dxfId="199" operator="containsText" priority="203" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D60)))</formula>
+    </cfRule>
+    <cfRule dxfId="198" operator="containsText" priority="204" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule dxfId="197" operator="containsText" priority="205" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D60)))</formula>
+    </cfRule>
+    <cfRule dxfId="196" operator="containsText" priority="206" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D60)))</formula>
+    </cfRule>
+    <cfRule dxfId="195" operator="containsText" priority="207" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E60">
+    <cfRule dxfId="194" operator="equal" priority="199" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="193" operator="equal" priority="200" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="192" operator="equal" priority="201" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule dxfId="191" operator="containsText" priority="193" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D61)))</formula>
+    </cfRule>
+    <cfRule dxfId="190" operator="containsText" priority="194" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D61)))</formula>
+    </cfRule>
+    <cfRule dxfId="189" operator="containsText" priority="195" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule dxfId="188" operator="containsText" priority="196" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D61)))</formula>
+    </cfRule>
+    <cfRule dxfId="187" operator="containsText" priority="197" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D61)))</formula>
+    </cfRule>
+    <cfRule dxfId="186" operator="containsText" priority="198" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61">
+    <cfRule dxfId="185" operator="equal" priority="190" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="184" operator="equal" priority="191" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="183" operator="equal" priority="192" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule dxfId="182" operator="containsText" priority="184" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D62)))</formula>
+    </cfRule>
+    <cfRule dxfId="181" operator="containsText" priority="185" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D62)))</formula>
+    </cfRule>
+    <cfRule dxfId="180" operator="containsText" priority="186" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule dxfId="179" operator="containsText" priority="187" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D62)))</formula>
+    </cfRule>
+    <cfRule dxfId="178" operator="containsText" priority="188" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D62)))</formula>
+    </cfRule>
+    <cfRule dxfId="177" operator="containsText" priority="189" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
+    <cfRule dxfId="176" operator="equal" priority="181" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="175" operator="equal" priority="182" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="174" operator="equal" priority="183" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:D64">
+    <cfRule dxfId="173" operator="containsText" priority="175" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D63)))</formula>
+    </cfRule>
+    <cfRule dxfId="172" operator="containsText" priority="176" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D63)))</formula>
+    </cfRule>
+    <cfRule dxfId="171" operator="containsText" priority="177" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:D64">
+    <cfRule dxfId="170" operator="containsText" priority="178" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D63)))</formula>
+    </cfRule>
+    <cfRule dxfId="169" operator="containsText" priority="179" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D63)))</formula>
+    </cfRule>
+    <cfRule dxfId="168" operator="containsText" priority="180" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63:E64">
+    <cfRule dxfId="167" operator="equal" priority="172" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="166" operator="equal" priority="173" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="165" operator="equal" priority="174" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule dxfId="164" operator="containsText" priority="166" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D65)))</formula>
+    </cfRule>
+    <cfRule dxfId="163" operator="containsText" priority="167" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D65)))</formula>
+    </cfRule>
+    <cfRule dxfId="162" operator="containsText" priority="168" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule dxfId="161" operator="containsText" priority="169" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D65)))</formula>
+    </cfRule>
+    <cfRule dxfId="160" operator="containsText" priority="170" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D65)))</formula>
+    </cfRule>
+    <cfRule dxfId="159" operator="containsText" priority="171" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule dxfId="158" operator="equal" priority="163" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="157" operator="equal" priority="164" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="156" operator="equal" priority="165" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule dxfId="155" operator="equal" priority="154" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="154" operator="equal" priority="155" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="153" operator="equal" priority="156" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule dxfId="152" operator="containsText" priority="157" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
+    </cfRule>
+    <cfRule dxfId="151" operator="containsText" priority="158" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
+    </cfRule>
+    <cfRule dxfId="150" operator="containsText" priority="159" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule dxfId="149" operator="containsText" priority="160" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
+    </cfRule>
+    <cfRule dxfId="148" operator="containsText" priority="161" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
+    </cfRule>
+    <cfRule dxfId="147" operator="containsText" priority="162" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule dxfId="146" operator="equal" priority="145" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="145" operator="equal" priority="146" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="144" operator="equal" priority="147" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule dxfId="143" operator="containsText" priority="148" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
+    </cfRule>
+    <cfRule dxfId="142" operator="containsText" priority="149" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
+    </cfRule>
+    <cfRule dxfId="141" operator="containsText" priority="150" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule dxfId="140" operator="containsText" priority="151" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
+    </cfRule>
+    <cfRule dxfId="139" operator="containsText" priority="152" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
+    </cfRule>
+    <cfRule dxfId="138" operator="containsText" priority="153" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule dxfId="137" operator="equal" priority="142" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="136" operator="equal" priority="143" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="135" operator="equal" priority="144" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule dxfId="134" operator="containsText" priority="136" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
+    </cfRule>
+    <cfRule dxfId="133" operator="containsText" priority="137" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
+    </cfRule>
+    <cfRule dxfId="132" operator="containsText" priority="138" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule dxfId="131" operator="containsText" priority="139" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
+    </cfRule>
+    <cfRule dxfId="130" operator="containsText" priority="140" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
+    </cfRule>
+    <cfRule dxfId="129" operator="containsText" priority="141" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
+    <cfRule dxfId="128" operator="equal" priority="133" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="127" operator="equal" priority="134" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="126" operator="equal" priority="135" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule dxfId="125" operator="containsText" priority="127" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="124" operator="containsText" priority="128" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="123" operator="containsText" priority="129" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule dxfId="122" operator="containsText" priority="130" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="121" operator="containsText" priority="131" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="120" operator="containsText" priority="132" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule dxfId="119" operator="equal" priority="124" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="118" operator="equal" priority="125" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="117" operator="equal" priority="126" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule dxfId="116" operator="containsText" priority="118" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D39)))</formula>
+    </cfRule>
+    <cfRule dxfId="115" operator="containsText" priority="119" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D39)))</formula>
+    </cfRule>
+    <cfRule dxfId="114" operator="containsText" priority="120" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule dxfId="113" operator="containsText" priority="121" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D39)))</formula>
+    </cfRule>
+    <cfRule dxfId="112" operator="containsText" priority="122" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D39)))</formula>
+    </cfRule>
+    <cfRule dxfId="111" operator="containsText" priority="123" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule dxfId="110" operator="equal" priority="115" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="109" operator="equal" priority="116" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="108" operator="equal" priority="117" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule dxfId="107" operator="containsText" priority="109" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D40)))</formula>
+    </cfRule>
+    <cfRule dxfId="106" operator="containsText" priority="110" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D40)))</formula>
+    </cfRule>
+    <cfRule dxfId="105" operator="containsText" priority="111" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule dxfId="104" operator="containsText" priority="112" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D40)))</formula>
+    </cfRule>
+    <cfRule dxfId="103" operator="containsText" priority="113" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D40)))</formula>
+    </cfRule>
+    <cfRule dxfId="102" operator="containsText" priority="114" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule dxfId="101" operator="equal" priority="106" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="100" operator="equal" priority="107" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="99" operator="equal" priority="108" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41:D43">
+    <cfRule dxfId="98" operator="containsText" priority="100" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D41)))</formula>
+    </cfRule>
+    <cfRule dxfId="97" operator="containsText" priority="101" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D41)))</formula>
+    </cfRule>
+    <cfRule dxfId="96" operator="containsText" priority="102" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41:D43">
+    <cfRule dxfId="95" operator="containsText" priority="103" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D41)))</formula>
+    </cfRule>
+    <cfRule dxfId="94" operator="containsText" priority="104" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D41)))</formula>
+    </cfRule>
+    <cfRule dxfId="93" operator="containsText" priority="105" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule dxfId="92" operator="equal" priority="97" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="91" operator="equal" priority="98" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="90" operator="equal" priority="99" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule dxfId="89" operator="equal" priority="94" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="88" operator="equal" priority="95" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="87" operator="equal" priority="96" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule dxfId="86" operator="equal" priority="85" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="85" operator="equal" priority="86" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="84" operator="equal" priority="87" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule dxfId="83" operator="containsText" priority="88" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="82" operator="containsText" priority="89" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="81" operator="containsText" priority="90" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule dxfId="80" operator="containsText" priority="91" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="79" operator="containsText" priority="92" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="78" operator="containsText" priority="93" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule dxfId="77" operator="containsText" priority="79" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D66)))</formula>
+    </cfRule>
+    <cfRule dxfId="76" operator="containsText" priority="80" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D66)))</formula>
+    </cfRule>
+    <cfRule dxfId="75" operator="containsText" priority="81" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule dxfId="74" operator="containsText" priority="82" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D66)))</formula>
+    </cfRule>
+    <cfRule dxfId="73" operator="containsText" priority="83" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D66)))</formula>
+    </cfRule>
+    <cfRule dxfId="72" operator="containsText" priority="84" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule dxfId="71" operator="equal" priority="76" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="70" operator="equal" priority="77" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="69" operator="equal" priority="78" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule dxfId="68" operator="containsText" priority="70" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D67)))</formula>
+    </cfRule>
+    <cfRule dxfId="67" operator="containsText" priority="71" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D67)))</formula>
+    </cfRule>
+    <cfRule dxfId="66" operator="containsText" priority="72" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule dxfId="65" operator="containsText" priority="73" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D67)))</formula>
+    </cfRule>
+    <cfRule dxfId="64" operator="containsText" priority="74" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D67)))</formula>
+    </cfRule>
+    <cfRule dxfId="63" operator="containsText" priority="75" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
+    <cfRule dxfId="62" operator="equal" priority="67" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="61" operator="equal" priority="68" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="60" operator="equal" priority="69" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule dxfId="59" operator="equal" priority="58" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="58" operator="equal" priority="59" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="57" operator="equal" priority="60" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule dxfId="56" operator="equal" priority="43" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="55" operator="equal" priority="44" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="54" operator="equal" priority="45" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46:D47">
+    <cfRule dxfId="53" operator="containsText" priority="49" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="52" operator="containsText" priority="50" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="51" operator="containsText" priority="51" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46:D47">
+    <cfRule dxfId="50" operator="containsText" priority="52" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="49" operator="containsText" priority="53" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="48" operator="containsText" priority="54" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule dxfId="47" operator="equal" priority="46" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="46" operator="equal" priority="47" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="45" operator="equal" priority="48" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule dxfId="44" operator="containsText" priority="37" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D68)))</formula>
+    </cfRule>
+    <cfRule dxfId="43" operator="containsText" priority="38" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D68)))</formula>
+    </cfRule>
+    <cfRule dxfId="42" operator="containsText" priority="39" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule dxfId="41" operator="containsText" priority="40" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D68)))</formula>
+    </cfRule>
+    <cfRule dxfId="40" operator="containsText" priority="41" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D68)))</formula>
+    </cfRule>
+    <cfRule dxfId="39" operator="containsText" priority="42" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule dxfId="38" operator="equal" priority="34" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="37" operator="equal" priority="35" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="36" operator="equal" priority="36" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69">
+    <cfRule dxfId="35" operator="containsText" priority="28" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D69)))</formula>
+    </cfRule>
+    <cfRule dxfId="34" operator="containsText" priority="29" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D69)))</formula>
+    </cfRule>
+    <cfRule dxfId="33" operator="containsText" priority="30" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69">
+    <cfRule dxfId="32" operator="containsText" priority="31" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D69)))</formula>
+    </cfRule>
+    <cfRule dxfId="31" operator="containsText" priority="32" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D69)))</formula>
+    </cfRule>
+    <cfRule dxfId="30" operator="containsText" priority="33" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule dxfId="29" operator="equal" priority="25" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="28" operator="equal" priority="26" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="27" operator="equal" priority="27" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule dxfId="26" operator="equal" priority="16" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="25" operator="equal" priority="17" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="24" operator="equal" priority="18" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule dxfId="23" operator="containsText" priority="10" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="235" priority="320" operator="containsText" text="Fail">
+    <cfRule dxfId="22" operator="containsText" priority="11" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="321" operator="containsText" text="Pass">
+    <cfRule dxfId="21" operator="containsText" priority="12" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D50">
-    <cfRule type="containsText" dxfId="233" priority="322" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D48">
+    <cfRule dxfId="20" operator="containsText" priority="13" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="323" operator="containsText" text="Fail">
+    <cfRule dxfId="19" operator="containsText" priority="14" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="231" priority="324" operator="containsText" text="Pass">
+    <cfRule dxfId="18" operator="containsText" priority="15" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E33">
-    <cfRule type="cellIs" dxfId="230" priority="238" operator="equal">
+  <conditionalFormatting sqref="E49">
+    <cfRule dxfId="17" operator="equal" priority="7" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="239" operator="equal">
+    <cfRule dxfId="16" operator="equal" priority="8" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="228" priority="240" operator="equal">
+    <cfRule dxfId="15" operator="equal" priority="9" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48:E50">
-    <cfRule type="cellIs" dxfId="227" priority="280" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="281" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="282" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E54">
-    <cfRule type="cellIs" dxfId="224" priority="193" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="223" priority="194" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="195" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D33">
-    <cfRule type="containsText" dxfId="221" priority="241" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="242" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="219" priority="243" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D33">
-    <cfRule type="containsText" dxfId="218" priority="244" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="245" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="246" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="containsText" dxfId="215" priority="223" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="224" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="225" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="containsText" dxfId="212" priority="226" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="227" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="228" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="209" priority="220" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="221" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="222" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="containsText" dxfId="206" priority="214" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="215" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="216" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="containsText" dxfId="203" priority="217" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="218" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="219" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="200" priority="211" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="212" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="213" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="containsText" dxfId="197" priority="205" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="206" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="207" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="containsText" dxfId="194" priority="208" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="209" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="210" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="191" priority="202" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="203" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="204" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="188" priority="196" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="197" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="198" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="185" priority="199" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="200" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="201" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="182" priority="187" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="188" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="189" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="179" priority="190" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="191" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="192" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E55">
-    <cfRule type="cellIs" dxfId="176" priority="184" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="185" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="186" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="173" priority="178" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="179" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="180" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="170" priority="181" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="182" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="183" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="167" priority="175" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="176" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="177" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="164" priority="169" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="170" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="171" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="161" priority="172" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="173" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="174" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" dxfId="158" priority="166" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="167" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="168" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="containsText" dxfId="155" priority="160" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="161" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="162" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="containsText" dxfId="152" priority="163" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="164" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="165" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
-    <cfRule type="cellIs" dxfId="149" priority="157" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="158" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="159" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="containsText" dxfId="146" priority="151" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="152" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="153" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="containsText" dxfId="143" priority="154" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="155" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="156" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="140" priority="148" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="149" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="150" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="containsText" dxfId="137" priority="142" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="143" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="144" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="containsText" dxfId="134" priority="145" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="146" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="147" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="131" priority="139" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="140" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="141" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61:D62">
-    <cfRule type="containsText" dxfId="128" priority="133" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="134" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="135" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D61)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61:D62">
-    <cfRule type="containsText" dxfId="125" priority="136" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="137" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="138" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D61)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E62">
-    <cfRule type="cellIs" dxfId="122" priority="130" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="131" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="132" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="containsText" dxfId="119" priority="124" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="125" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="126" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="containsText" dxfId="116" priority="127" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="128" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="129" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
-    <cfRule type="cellIs" dxfId="113" priority="121" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="122" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="123" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="110" priority="112" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="113" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="114" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="containsText" dxfId="107" priority="115" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="116" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="117" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="containsText" dxfId="104" priority="118" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="119" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="120" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="101" priority="103" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="104" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="105" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="98" priority="106" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="107" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="108" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="95" priority="109" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="110" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="111" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="92" priority="100" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="101" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="102" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="95" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="96" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="86" priority="97" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="98" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="99" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="83" priority="91" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="92" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="93" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="80" priority="85" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="86" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="87" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="77" priority="88" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="89" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="90" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="74" priority="82" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="83" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="84" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="71" priority="76" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="77" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="78" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="68" priority="79" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="80" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="81" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="65" priority="73" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="74" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="75" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="62" priority="67" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="68" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="69" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="59" priority="70" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="71" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="72" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="65" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="66" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41:D43">
-    <cfRule type="containsText" dxfId="53" priority="58" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41:D43">
-    <cfRule type="containsText" dxfId="50" priority="61" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="62" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="63" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="56" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="57" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="54" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="38" priority="46" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="48" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="35" priority="49" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="50" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="51" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="39" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="41" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="42" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="36" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="32" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="33" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46:D47">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46:D47">
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
-      <formula>"Low"</formula>
+  <conditionalFormatting sqref="D49">
+    <cfRule dxfId="11" operator="containsText" priority="1" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="10" operator="containsText" priority="2" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="9" operator="containsText" priority="3" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule dxfId="5" operator="containsText" priority="4" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="4" operator="containsText" priority="5" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="3" operator="containsText" priority="6" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+    <dataValidation showDropDown="1" showErrorMessage="1" showInputMessage="1" sqref="C1">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C65">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="C2:C69" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E65">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E69" type="list">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="D3" pane="bottomLeft" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="19" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="1025" width="19" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="6" max="1025" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6708,9 +7147,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="javascript:srcUp(%27%2F0054x000001Z8z4%3Fnoredirect%3D1%26isUserEntityOverride%3D1%26isdtp%3Dp1%27);"/>
+    <hyperlink display="javascript:srcUp(%27%2F0054x000001Z8z4%3Fnoredirect%3D1%26isUserEntityOverride%3D1%26isdtp%3Dp1%27);" r:id="rId1" ref="E3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>